<commit_message>
debug the descriptive data
</commit_message>
<xml_diff>
--- a/Refinitiv/Analysis/AU/AU_Descriptive Statistics.xlsx
+++ b/Refinitiv/Analysis/AU/AU_Descriptive Statistics.xlsx
@@ -824,66 +824,6 @@
       <c r="D3" t="n">
         <v>404</v>
       </c>
-      <c r="G3" t="n">
-        <v>2096</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1593</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2095</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2088</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1647</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1647</v>
-      </c>
-      <c r="M3" t="n">
-        <v>2096</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2096</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1738</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1692</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1514</v>
-      </c>
-      <c r="R3" t="n">
-        <v>387</v>
-      </c>
-      <c r="S3" t="n">
-        <v>396</v>
-      </c>
-      <c r="T3" t="n">
-        <v>2317</v>
-      </c>
-      <c r="U3" t="n">
-        <v>402</v>
-      </c>
-      <c r="V3" t="n">
-        <v>2322</v>
-      </c>
-      <c r="W3" t="n">
-        <v>401</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>1514</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>2206</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>1692</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -901,66 +841,6 @@
           <t>ALD.AX</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>43.7233176005385</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>31.6623169493983</v>
-      </c>
-      <c r="J4" t="n">
-        <v>26.8868640850417</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2291.954696832466</v>
-      </c>
-      <c r="N4" t="n">
-        <v>83587.112458841</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="P4" t="n">
-        <v>12.689070377</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>15.937280599</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>10.649415841</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>6927738083.57191</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.0627459618212875</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>0.520797368</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0.3726599229662262</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -974,66 +854,6 @@
       <c r="D5" t="n">
         <v>6</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>450</v>
-      </c>
-      <c r="I5" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" t="n">
-        <v>450</v>
-      </c>
-      <c r="L5" t="n">
-        <v>450</v>
-      </c>
-      <c r="M5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="n">
-        <v>8</v>
-      </c>
-      <c r="P5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" t="n">
-        <v>106</v>
-      </c>
-      <c r="S5" t="n">
-        <v>50</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" t="n">
-        <v>17</v>
-      </c>
-      <c r="V5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" t="n">
-        <v>22</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1050,9 +870,63 @@
       <c r="F6" t="n">
         <v>2019.464435146444</v>
       </c>
+      <c r="G6" t="n">
+        <v>40.60432299793592</v>
+      </c>
+      <c r="H6" t="n">
+        <v>26.44206943848964</v>
+      </c>
+      <c r="I6" t="n">
+        <v>42.81318016591187</v>
+      </c>
+      <c r="J6" t="n">
+        <v>49.4768054228887</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1566.752522467704</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1653.625127759921</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2425.883965411414</v>
+      </c>
+      <c r="N6" t="n">
+        <v>124379.4953272435</v>
+      </c>
+      <c r="O6" t="n">
+        <v>9.111649313701808</v>
+      </c>
+      <c r="P6" t="n">
+        <v>37.97458256181991</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>64.48632034329007</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1.224350214138081</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1.08688534414102</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-2.897813695950064</v>
+      </c>
+      <c r="U6" t="n">
+        <v>49.69170728029123</v>
+      </c>
+      <c r="V6" t="n">
+        <v>3925786798.274295</v>
+      </c>
+      <c r="W6" t="n">
+        <v>45.08999531772432</v>
+      </c>
       <c r="X6" t="n">
         <v>-0.03787168728730674</v>
       </c>
+      <c r="Y6" t="n">
+        <v>0.08688650894950616</v>
+      </c>
       <c r="Z6" t="n">
         <v>0.08534120446916728</v>
       </c>
@@ -1062,6 +936,9 @@
       <c r="AB6" t="n">
         <v>2.346574424571005e-18</v>
       </c>
+      <c r="AC6" t="n">
+        <v>820.1013819865034</v>
+      </c>
       <c r="AD6" t="n">
         <v>894.9867776600169</v>
       </c>
@@ -1071,6 +948,9 @@
       <c r="AF6" t="n">
         <v>-1.288382113798912e-17</v>
       </c>
+      <c r="AG6" t="n">
+        <v>29.22209177644399</v>
+      </c>
       <c r="AH6" t="n">
         <v>34.65582866586207</v>
       </c>
@@ -1111,9 +991,63 @@
       <c r="F7" t="n">
         <v>1.693866139305341</v>
       </c>
+      <c r="G7" t="n">
+        <v>21.02235277283804</v>
+      </c>
+      <c r="H7" t="n">
+        <v>26.41242032004845</v>
+      </c>
+      <c r="I7" t="n">
+        <v>22.62590860512981</v>
+      </c>
+      <c r="J7" t="n">
+        <v>22.78286139374379</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2032.941644460481</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2021.725719384686</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2017.510936805265</v>
+      </c>
+      <c r="N7" t="n">
+        <v>160183.2908472984</v>
+      </c>
+      <c r="O7" t="n">
+        <v>23.05367796400245</v>
+      </c>
+      <c r="P7" t="n">
+        <v>351.7387432869111</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>521.1813266575277</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.699713089277471</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.5992760263355361</v>
+      </c>
+      <c r="T7" t="n">
+        <v>32.53274329231496</v>
+      </c>
+      <c r="U7" t="n">
+        <v>26.38298018277067</v>
+      </c>
+      <c r="V7" t="n">
+        <v>13096910101.57792</v>
+      </c>
+      <c r="W7" t="n">
+        <v>25.87297132514584</v>
+      </c>
       <c r="X7" t="n">
         <v>1.186279100408466</v>
       </c>
+      <c r="Y7" t="n">
+        <v>0.3675053469566921</v>
+      </c>
       <c r="Z7" t="n">
         <v>0.06496678944564827</v>
       </c>
@@ -1123,6 +1057,9 @@
       <c r="AB7" t="n">
         <v>0.978283698818206</v>
       </c>
+      <c r="AC7" t="n">
+        <v>21714.27698207647</v>
+      </c>
       <c r="AD7" t="n">
         <v>2505.990337549306</v>
       </c>
@@ -1132,6 +1069,9 @@
       <c r="AF7" t="n">
         <v>0.9851505174084382</v>
       </c>
+      <c r="AG7" t="n">
+        <v>397.5019453200886</v>
+      </c>
       <c r="AH7" t="n">
         <v>73.57194553369315</v>
       </c>
@@ -1172,9 +1112,63 @@
       <c r="F8" t="n">
         <v>2017</v>
       </c>
+      <c r="G8" t="n">
+        <v>2.16036717202278</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.02448250499106</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.03274559193954</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>6.351908046707315</v>
+      </c>
+      <c r="N8" t="n">
+        <v>10.08283610702105</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.008564348508246999</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.07263964552878199</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-1.4452784998966</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-0.258896562661341</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-842.151252707</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>1866576.53527322</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
       <c r="X8" t="n">
         <v>-7.834947164649852</v>
       </c>
+      <c r="Y8" t="n">
+        <v>6.063618290258458e-05</v>
+      </c>
       <c r="Z8" t="n">
         <v>0.005922571980311104</v>
       </c>
@@ -1184,6 +1178,9 @@
       <c r="AB8" t="n">
         <v>-2.054839772336394</v>
       </c>
+      <c r="AC8" t="n">
+        <v>0.0006432620052380001</v>
+      </c>
       <c r="AD8" t="n">
         <v>1.141065638731942</v>
       </c>
@@ -1193,6 +1190,9 @@
       <c r="AF8" t="n">
         <v>-1.822603921518096</v>
       </c>
+      <c r="AG8" t="n">
+        <v>0.0001714480194709703</v>
+      </c>
       <c r="AH8" t="n">
         <v>3.646313867832114</v>
       </c>
@@ -1233,9 +1233,63 @@
       <c r="F9" t="n">
         <v>2018</v>
       </c>
+      <c r="G9" t="n">
+        <v>23.48044685127255</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2.17108773862599</v>
+      </c>
+      <c r="I9" t="n">
+        <v>25.17719770829013</v>
+      </c>
+      <c r="J9" t="n">
+        <v>31.34766011627065</v>
+      </c>
+      <c r="K9" t="n">
+        <v>35.61502562195389</v>
+      </c>
+      <c r="L9" t="n">
+        <v>54.84232474422455</v>
+      </c>
+      <c r="M9" t="n">
+        <v>786.8455343023638</v>
+      </c>
+      <c r="N9" t="n">
+        <v>12945.50886007589</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="P9" t="n">
+        <v>6.844607536320606</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>10.71958658975</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.83862821426832</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.6661071171265258</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-5.6834794496</v>
+      </c>
+      <c r="U9" t="n">
+        <v>31.0969492849966</v>
+      </c>
+      <c r="V9" t="n">
+        <v>198630076.2029462</v>
+      </c>
+      <c r="W9" t="n">
+        <v>27.3476192806246</v>
+      </c>
       <c r="X9" t="n">
         <v>-0.3364722366212129</v>
       </c>
+      <c r="Y9" t="n">
+        <v>0.03027429419420288</v>
+      </c>
       <c r="Z9" t="n">
         <v>0.05140477157534346</v>
       </c>
@@ -1245,6 +1299,9 @@
       <c r="AB9" t="n">
         <v>-0.568832611611249</v>
       </c>
+      <c r="AC9" t="n">
+        <v>1.159136290676698</v>
+      </c>
       <c r="AD9" t="n">
         <v>6.965754436555632</v>
       </c>
@@ -1254,6 +1311,9 @@
       <c r="AF9" t="n">
         <v>-0.303830129962721</v>
       </c>
+      <c r="AG9" t="n">
+        <v>1.375437490318808</v>
+      </c>
       <c r="AH9" t="n">
         <v>7.919825298913707</v>
       </c>
@@ -1294,9 +1354,63 @@
       <c r="F10" t="n">
         <v>2019</v>
       </c>
+      <c r="G10" t="n">
+        <v>37.94902687367665</v>
+      </c>
+      <c r="H10" t="n">
+        <v>18.56011789730495</v>
+      </c>
+      <c r="I10" t="n">
+        <v>40.70015947858415</v>
+      </c>
+      <c r="J10" t="n">
+        <v>48.56598142226279</v>
+      </c>
+      <c r="K10" t="n">
+        <v>622.5531833710047</v>
+      </c>
+      <c r="L10" t="n">
+        <v>746.8600732776019</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1899.320061502804</v>
+      </c>
+      <c r="N10" t="n">
+        <v>54651.48072600651</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2.7190094475</v>
+      </c>
+      <c r="P10" t="n">
+        <v>12.9509082136824</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>19.1603426405092</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1.17109985413391</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1.00882716143141</v>
+      </c>
+      <c r="T10" t="n">
+        <v>3.325495419</v>
+      </c>
+      <c r="U10" t="n">
+        <v>42.7114602373328</v>
+      </c>
+      <c r="V10" t="n">
+        <v>637823291.1727235</v>
+      </c>
+      <c r="W10" t="n">
+        <v>38.8014765635393</v>
+      </c>
       <c r="X10" t="n">
         <v>-0.006006245643133191</v>
       </c>
+      <c r="Y10" t="n">
+        <v>0.05219115266495034</v>
+      </c>
       <c r="Z10" t="n">
         <v>0.06951906463529176</v>
       </c>
@@ -1306,6 +1420,9 @@
       <c r="AB10" t="n">
         <v>-0.2242252464039884</v>
       </c>
+      <c r="AC10" t="n">
+        <v>3.011525833169725</v>
+      </c>
       <c r="AD10" t="n">
         <v>18.90396939270079</v>
       </c>
@@ -1315,6 +1432,9 @@
       <c r="AF10" t="n">
         <v>-0.216473407089317</v>
       </c>
+      <c r="AG10" t="n">
+        <v>3.387357080809172</v>
+      </c>
       <c r="AH10" t="n">
         <v>11.68677436740997</v>
       </c>
@@ -1355,9 +1475,63 @@
       <c r="F11" t="n">
         <v>2021</v>
       </c>
+      <c r="G11" t="n">
+        <v>55.8085593657264</v>
+      </c>
+      <c r="H11" t="n">
+        <v>44.71878761674657</v>
+      </c>
+      <c r="I11" t="n">
+        <v>59.69642665709583</v>
+      </c>
+      <c r="J11" t="n">
+        <v>67.430836296219</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2443.749869229816</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2709.88651757683</v>
+      </c>
+      <c r="M11" t="n">
+        <v>3471.141985412267</v>
+      </c>
+      <c r="N11" t="n">
+        <v>173821.0829215753</v>
+      </c>
+      <c r="O11" t="n">
+        <v>7.498422</v>
+      </c>
+      <c r="P11" t="n">
+        <v>23.7289934845</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>33.0313253835</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.59915043957711</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1.44171485602766</v>
+      </c>
+      <c r="T11" t="n">
+        <v>8.438454714300001</v>
+      </c>
+      <c r="U11" t="n">
+        <v>61.7452197879924</v>
+      </c>
+      <c r="V11" t="n">
+        <v>2200145121.368382</v>
+      </c>
+      <c r="W11" t="n">
+        <v>55.8491649443871</v>
+      </c>
       <c r="X11" t="n">
         <v>0.2808765081798253</v>
       </c>
+      <c r="Y11" t="n">
+        <v>0.09328730866713247</v>
+      </c>
       <c r="Z11" t="n">
         <v>0.09844668329108781</v>
       </c>
@@ -1367,6 +1541,9 @@
       <c r="AB11" t="n">
         <v>0.2703982942800119</v>
       </c>
+      <c r="AC11" t="n">
+        <v>10.34662760911812</v>
+      </c>
       <c r="AD11" t="n">
         <v>734.1691505937421</v>
       </c>
@@ -1376,6 +1553,9 @@
       <c r="AF11" t="n">
         <v>-0.113196765958869</v>
       </c>
+      <c r="AG11" t="n">
+        <v>8.395804536415389</v>
+      </c>
       <c r="AH11" t="n">
         <v>24.65249255640071</v>
       </c>
@@ -1416,9 +1596,63 @@
       <c r="F12" t="n">
         <v>2022</v>
       </c>
+      <c r="G12" t="n">
+        <v>90.8780085125484</v>
+      </c>
+      <c r="H12" t="n">
+        <v>96.3711567124062</v>
+      </c>
+      <c r="I12" t="n">
+        <v>96.9258279083044</v>
+      </c>
+      <c r="J12" t="n">
+        <v>98.1338048317139</v>
+      </c>
+      <c r="K12" t="n">
+        <v>8935.80148567679</v>
+      </c>
+      <c r="L12" t="n">
+        <v>8780.787176347189</v>
+      </c>
+      <c r="M12" t="n">
+        <v>8892.806589289692</v>
+      </c>
+      <c r="N12" t="n">
+        <v>750544.426426754</v>
+      </c>
+      <c r="O12" t="n">
+        <v>290.72</v>
+      </c>
+      <c r="P12" t="n">
+        <v>13907.3775699265</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>16491.8032786885</v>
+      </c>
+      <c r="R12" t="n">
+        <v>4.88895043111182</v>
+      </c>
+      <c r="S12" t="n">
+        <v>3.77451006704652</v>
+      </c>
+      <c r="T12" t="n">
+        <v>177.6931560046</v>
+      </c>
+      <c r="U12" t="n">
+        <v>245.309152184057</v>
+      </c>
+      <c r="V12" t="n">
+        <v>157485039972.121</v>
+      </c>
+      <c r="W12" t="n">
+        <v>265.883848205148</v>
+      </c>
       <c r="X12" t="n">
         <v>8.036391633808032</v>
       </c>
+      <c r="Y12" t="n">
+        <v>13.76658700246231</v>
+      </c>
       <c r="Z12" t="n">
         <v>0.5102882823758979</v>
       </c>
@@ -1428,6 +1662,9 @@
       <c r="AB12" t="n">
         <v>5.715505624526492</v>
       </c>
+      <c r="AC12" t="n">
+        <v>1010044.90447419</v>
+      </c>
       <c r="AD12" t="n">
         <v>12255.67173969096</v>
       </c>
@@ -1436,6 +1673,9 @@
       </c>
       <c r="AF12" t="n">
         <v>9.340512031102113</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>15444.73098747262</v>
       </c>
       <c r="AH12" t="n">
         <v>354.8276216025998</v>

</xml_diff>